<commit_message>
Excel sheet impoting and assigning
</commit_message>
<xml_diff>
--- a/src/excelSheetIO/RosterSheet.xlsx
+++ b/src/excelSheetIO/RosterSheet.xlsx
@@ -19,7 +19,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
   <numFmts count="2">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -411,6 +411,12 @@
       <c r="A3" t="str">
         <v>Collins Street</v>
       </c>
+      <c r="B3" t="str">
+        <v>Class Room</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Class Room</v>
+      </c>
       <c r="E3" t="str">
         <v>P123</v>
       </c>
@@ -419,19 +425,34 @@
       <c r="A4" t="str">
         <v>DWH</v>
       </c>
+      <c r="B4" t="str">
+        <v>Offsite</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Offsite</v>
+      </c>
       <c r="E4" t="str">
         <v>P456</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Other</v>
+        <v>eClass</v>
+      </c>
+      <c r="B5" t="str">
+        <v>eClass</v>
+      </c>
+      <c r="C5" t="str">
+        <v>eClass</v>
       </c>
       <c r="E5" t="str">
         <v>DHD</v>
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="str">
+        <v>Other</v>
+      </c>
       <c r="E6" t="str">
         <v>HHI</v>
       </c>
@@ -501,7 +522,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Contact Information</v>
+        <v>School Contact Information</v>
       </c>
     </row>
     <row r="2">
@@ -531,14 +552,46 @@
       <c r="C3" t="str">
         <v>fjames@doxa.org.au</v>
       </c>
-      <c r="D3" t="str">
-        <v>90468200</v>
+      <c r="D3">
+        <v>490468200</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Toby Wetherell</v>
+      </c>
+      <c r="B4" t="str">
+        <v>School of Melbourne</v>
+      </c>
+      <c r="C4" t="str">
+        <v>t.wetherell@gmail.com.au</v>
+      </c>
+      <c r="D4">
+        <v>467288231</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Sasha Murray</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Melbourne High</v>
+      </c>
+      <c r="C5" t="str">
+        <v>s.murray@gmail.com</v>
+      </c>
+      <c r="D5">
+        <v>472944823</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:E24"/>
@@ -548,7 +601,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -576,24 +629,27 @@
         <v>Trained?</v>
       </c>
       <c r="H1" t="str">
+        <v>Reliable?</v>
+      </c>
+      <c r="I1" t="str">
         <v>Monday</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>Tuesday</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>Wednesday</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>Thursday</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>Friday</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>Saturday</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>Sunday</v>
       </c>
     </row>
@@ -620,34 +676,85 @@
         <v>Yes</v>
       </c>
       <c r="H2" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="I2" t="str">
         <v>Morning</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <v>Afternoon</v>
       </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <v>Morning and Afternoon</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <v>Morning</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <v>Afternoon</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <v>Morning and Afternoon</v>
       </c>
-      <c r="N2" t="str">
+      <c r="O2" t="str">
         <v>Morning</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Guest Speaker</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Test</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Mcgrath</v>
+      </c>
+      <c r="D3" t="str">
+        <v>t.mcgrath@gmail.com</v>
+      </c>
+      <c r="E3">
+        <v>472844295</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Sydney</v>
+      </c>
+      <c r="G3" t="str">
+        <v>No</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Morning and Afternoon</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Afternoon</v>
+      </c>
+      <c r="K3" t="str">
+        <v>Morning and Afternoon</v>
+      </c>
+      <c r="L3" t="str">
+        <v>Unavailable</v>
+      </c>
+      <c r="M3" t="str">
+        <v>Unavailable</v>
+      </c>
+      <c r="N3" t="str">
+        <v>Unavailable</v>
+      </c>
+      <c r="O3" t="str">
+        <v>Unavailable</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N49"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O49"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -729,7 +836,7 @@
         <v>January</v>
       </c>
       <c r="C2" t="str">
-        <v>Feb</v>
+        <v>Monday</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -748,7 +855,7 @@
         <v>Collins Street</v>
       </c>
       <c r="I2" t="str">
-        <v>DWH</v>
+        <v>n.a</v>
       </c>
       <c r="J2" t="str">
         <v>DHDe</v>
@@ -763,28 +870,28 @@
         <v>Fran James</v>
       </c>
       <c r="N2" t="str">
-        <f>INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M2,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0))</f>
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M2,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
         <v>Doxa University Pathways</v>
       </c>
       <c r="O2" t="str">
-        <f>INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M2,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0))</f>
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M2,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
         <v>fjames@doxa.org.au</v>
       </c>
-      <c r="P2" t="str">
-        <f>INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M2,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0))</f>
-        <v>90468200</v>
+      <c r="P2">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M2,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v>490468200</v>
       </c>
       <c r="Q2">
-        <f>INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M2,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0))</f>
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M2,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
         <v>0</v>
       </c>
       <c r="R2" t="str">
-        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A2,RosterOutput!A2:$A$10000,0),1),Pending)</f>
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A2,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
         <v>Seb Gould</v>
       </c>
-      <c r="S2" t="e">
-        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A2,RosterOutput!$A2:B$10000,0),1),Pending)</f>
-        <v>#NAME?</v>
+      <c r="S2" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A2,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Richard Fontein</v>
       </c>
     </row>
     <row r="3">
@@ -795,8 +902,62 @@
       <c r="B3" t="str">
         <v>January</v>
       </c>
+      <c r="C3" t="str">
+        <v>Tuesday</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
       <c r="E3" t="str">
         <f>IF(COUNTIF(RosterOutput!A3:$A$1000,Melbourne!A3)&gt;1,"Rostered","Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="F3">
+        <v>0.625</v>
+      </c>
+      <c r="G3">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Other</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Melbourne High</v>
+      </c>
+      <c r="J3" t="str">
+        <v>P456</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3" t="str">
+        <v>Sasha Murray</v>
+      </c>
+      <c r="N3" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M3,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v>Melbourne High</v>
+      </c>
+      <c r="O3" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M3,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v>s.murray@gmail.com</v>
+      </c>
+      <c r="P3">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M3,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v>472944823</v>
+      </c>
+      <c r="Q3">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M3,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v>0</v>
+      </c>
+      <c r="R3" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A3,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S3" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A3,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
         <v>Pending</v>
       </c>
     </row>
@@ -812,6 +973,30 @@
         <f>IF(COUNTIF(RosterOutput!A4:$A$1000,Melbourne!A4)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N4" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M4,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O4" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M4,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P4" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M4,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q4" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M4,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R4" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A4,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S4" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A4,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -825,6 +1010,30 @@
         <f>IF(COUNTIF(RosterOutput!A5:$A$1000,Melbourne!A5)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N5" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M5,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O5" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M5,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P5" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M5,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q5" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M5,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R5" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A5,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S5" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A5,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -838,6 +1047,30 @@
         <f>IF(COUNTIF(RosterOutput!A6:$A$1000,Melbourne!A6)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N6" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M6,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O6" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M6,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P6" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M6,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q6" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M6,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R6" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A6,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S6" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A6,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -851,8 +1084,29 @@
         <f>IF(COUNTIF(RosterOutput!A7:$A$1000,Melbourne!A7)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
-      <c r="J7" t="str">
-        <v xml:space="preserve"> </v>
+      <c r="N7" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M7,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M7,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P7" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M7,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q7" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M7,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R7" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A7,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S7" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A7,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
       </c>
     </row>
     <row r="8">
@@ -867,6 +1121,30 @@
         <f>IF(COUNTIF(RosterOutput!A8:$A$1000,Melbourne!A8)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N8" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M8,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O8" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M8,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P8" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M8,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q8" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M8,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R8" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A8,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S8" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A8,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -880,6 +1158,30 @@
         <f>IF(COUNTIF(RosterOutput!A9:$A$1000,Melbourne!A9)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N9" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M9,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O9" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M9,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P9" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M9,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q9" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M9,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R9" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A9,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S9" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A9,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -893,6 +1195,30 @@
         <f>IF(COUNTIF(RosterOutput!A10:$A$1000,Melbourne!A10)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N10" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M10,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O10" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M10,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P10" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M10,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q10" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M10,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R10" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A10,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S10" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A10,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -906,6 +1232,30 @@
         <f>IF(COUNTIF(RosterOutput!A11:$A$1000,Melbourne!A11)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N11" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M11,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O11" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M11,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P11" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M11,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q11" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M11,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R11" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A11,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S11" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A11,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -919,6 +1269,30 @@
         <f>IF(COUNTIF(RosterOutput!A12:$A$1000,Melbourne!A12)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N12" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M12,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O12" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M12,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P12" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M12,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q12" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M12,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R12" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A12,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S12" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A12,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -932,6 +1306,30 @@
         <f>IF(COUNTIF(RosterOutput!A13:$A$1000,Melbourne!A13)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N13" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M13,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O13" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M13,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P13" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M13,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q13" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M13,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R13" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A13,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S13" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A13,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -945,6 +1343,30 @@
         <f>IF(COUNTIF(RosterOutput!A14:$A$1000,Melbourne!A14)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N14" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M14,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O14" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M14,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P14" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M14,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q14" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M14,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R14" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A14,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S14" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A14,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -958,6 +1380,30 @@
         <f>IF(COUNTIF(RosterOutput!A15:$A$1000,Melbourne!A15)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N15" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M15,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O15" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M15,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P15" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M15,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q15" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M15,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R15" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A15,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S15" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A15,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -971,6 +1417,30 @@
         <f>IF(COUNTIF(RosterOutput!A16:$A$1000,Melbourne!A16)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N16" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M16,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O16" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M16,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P16" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M16,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q16" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M16,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R16" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A16,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S16" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A16,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -984,6 +1454,30 @@
         <f>IF(COUNTIF(RosterOutput!A17:$A$1000,Melbourne!A17)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N17" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M17,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O17" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M17,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P17" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M17,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q17" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M17,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R17" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A17,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S17" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A17,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -997,6 +1491,30 @@
         <f>IF(COUNTIF(RosterOutput!A18:$A$1000,Melbourne!A18)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N18" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M18,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O18" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M18,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P18" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M18,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q18" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M18,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R18" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A18,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S18" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A18,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -1010,6 +1528,30 @@
         <f>IF(COUNTIF(RosterOutput!A19:$A$1000,Melbourne!A19)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N19" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M19,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O19" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M19,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P19" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M19,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q19" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M19,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R19" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A19,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S19" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A19,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -1023,6 +1565,30 @@
         <f>IF(COUNTIF(RosterOutput!A20:$A$1000,Melbourne!A20)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N20" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M20,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O20" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M20,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P20" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M20,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q20" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M20,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R20" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A20,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S20" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A20,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -1036,6 +1602,30 @@
         <f>IF(COUNTIF(RosterOutput!A21:$A$1000,Melbourne!A21)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N21" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M21,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O21" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M21,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P21" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M21,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q21" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M21,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R21" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A21,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S21" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A21,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -1049,6 +1639,30 @@
         <f>IF(COUNTIF(RosterOutput!A22:$A$1000,Melbourne!A22)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N22" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M22,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O22" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M22,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P22" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M22,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q22" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M22,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R22" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A22,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S22" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A22,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -1062,6 +1676,30 @@
         <f>IF(COUNTIF(RosterOutput!A23:$A$1000,Melbourne!A23)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N23" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M23,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O23" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M23,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P23" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M23,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q23" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M23,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R23" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A23,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S23" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A23,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -1075,6 +1713,30 @@
         <f>IF(COUNTIF(RosterOutput!A24:$A$1000,Melbourne!A24)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N24" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M24,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O24" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M24,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P24" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M24,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q24" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M24,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R24" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A24,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S24" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A24,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -1088,6 +1750,30 @@
         <f>IF(COUNTIF(RosterOutput!A25:$A$1000,Melbourne!A25)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N25" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M25,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O25" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M25,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P25" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M25,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q25" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M25,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R25" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A25,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S25" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A25,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -1101,6 +1787,30 @@
         <f>IF(COUNTIF(RosterOutput!A26:$A$1000,Melbourne!A26)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N26" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M26,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O26" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M26,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P26" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M26,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q26" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M26,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R26" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A26,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S26" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A26,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -1114,6 +1824,30 @@
         <f>IF(COUNTIF(RosterOutput!A27:$A$1000,Melbourne!A27)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N27" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M27,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O27" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M27,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P27" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M27,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q27" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M27,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R27" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A27,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S27" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A27,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -1127,6 +1861,30 @@
         <f>IF(COUNTIF(RosterOutput!A28:$A$1000,Melbourne!A28)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N28" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M28,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O28" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M28,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P28" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M28,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q28" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M28,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R28" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A28,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S28" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A28,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -1140,6 +1898,30 @@
         <f>IF(COUNTIF(RosterOutput!A29:$A$1000,Melbourne!A29)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N29" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M29,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O29" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M29,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P29" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M29,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q29" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M29,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R29" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A29,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S29" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A29,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -1153,6 +1935,30 @@
         <f>IF(COUNTIF(RosterOutput!A30:$A$1000,Melbourne!A30)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N30" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M30,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O30" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M30,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P30" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M30,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q30" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M30,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R30" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A30,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S30" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A30,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -1166,6 +1972,30 @@
         <f>IF(COUNTIF(RosterOutput!A31:$A$1000,Melbourne!A31)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N31" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M31,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O31" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M31,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P31" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M31,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q31" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M31,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R31" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A31,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S31" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A31,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -1179,6 +2009,30 @@
         <f>IF(COUNTIF(RosterOutput!A32:$A$1000,Melbourne!A32)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N32" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M32,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O32" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M32,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P32" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M32,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q32" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M32,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R32" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A32,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S32" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A32,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -1192,6 +2046,30 @@
         <f>IF(COUNTIF(RosterOutput!A33:$A$1000,Melbourne!A33)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N33" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M33,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O33" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M33,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P33" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M33,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q33" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M33,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R33" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A33,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S33" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A33,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -1205,6 +2083,30 @@
         <f>IF(COUNTIF(RosterOutput!A34:$A$1000,Melbourne!A34)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N34" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M34,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O34" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M34,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P34" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M34,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q34" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M34,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R34" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A34,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S34" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A34,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -1218,6 +2120,30 @@
         <f>IF(COUNTIF(RosterOutput!A35:$A$1000,Melbourne!A35)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N35" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M35,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O35" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M35,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P35" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M35,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q35" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M35,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R35" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A35,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S35" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A35,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -1231,6 +2157,30 @@
         <f>IF(COUNTIF(RosterOutput!A36:$A$1000,Melbourne!A36)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N36" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M36,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O36" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M36,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P36" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M36,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q36" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M36,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R36" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A36,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S36" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A36,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -1244,6 +2194,30 @@
         <f>IF(COUNTIF(RosterOutput!A37:$A$1000,Melbourne!A37)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N37" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M37,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O37" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M37,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P37" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M37,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q37" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M37,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R37" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A37,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S37" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A37,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -1257,6 +2231,30 @@
         <f>IF(COUNTIF(RosterOutput!A38:$A$1000,Melbourne!A38)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N38" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M38,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O38" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M38,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P38" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M38,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q38" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M38,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R38" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A38,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S38" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A38,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -1270,6 +2268,30 @@
         <f>IF(COUNTIF(RosterOutput!A39:$A$1000,Melbourne!A39)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N39" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M39,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O39" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M39,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P39" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M39,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q39" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M39,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R39" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A39,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S39" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A39,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -1283,6 +2305,30 @@
         <f>IF(COUNTIF(RosterOutput!A40:$A$1000,Melbourne!A40)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N40" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M40,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O40" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M40,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P40" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M40,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q40" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M40,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R40" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A40,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S40" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A40,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -1296,6 +2342,30 @@
         <f>IF(COUNTIF(RosterOutput!A41:$A$1000,Melbourne!A41)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N41" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M41,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O41" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M41,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P41" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M41,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q41" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M41,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R41" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A41,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S41" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A41,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -1309,6 +2379,30 @@
         <f>IF(COUNTIF(RosterOutput!A42:$A$1000,Melbourne!A42)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N42" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M42,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O42" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M42,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P42" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M42,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q42" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M42,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R42" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A42,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S42" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A42,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -1322,6 +2416,30 @@
         <f>IF(COUNTIF(RosterOutput!A43:$A$1000,Melbourne!A43)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N43" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M43,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O43" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M43,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P43" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M43,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q43" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M43,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R43" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A43,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S43" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A43,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -1335,6 +2453,30 @@
         <f>IF(COUNTIF(RosterOutput!A44:$A$1000,Melbourne!A44)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N44" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M44,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O44" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M44,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P44" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M44,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q44" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M44,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R44" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A44,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S44" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A44,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -1348,6 +2490,30 @@
         <f>IF(COUNTIF(RosterOutput!A45:$A$1000,Melbourne!A45)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N45" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M45,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O45" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M45,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P45" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M45,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q45" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M45,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R45" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A45,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S45" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A45,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -1361,6 +2527,30 @@
         <f>IF(COUNTIF(RosterOutput!A46:$A$1000,Melbourne!A46)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N46" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M46,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O46" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M46,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P46" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M46,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q46" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M46,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R46" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A46,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S46" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A46,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -1374,6 +2564,30 @@
         <f>IF(COUNTIF(RosterOutput!A47:$A$1000,Melbourne!A47)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N47" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M47,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O47" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M47,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P47" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M47,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q47" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M47,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R47" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A47,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S47" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A47,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -1387,6 +2601,30 @@
         <f>IF(COUNTIF(RosterOutput!A48:$A$1000,Melbourne!A48)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N48" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M48,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O48" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M48,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P48" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M48,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q48" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M48,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R48" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A48,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S48" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A48,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -1400,6 +2638,30 @@
         <f>IF(COUNTIF(RosterOutput!A49:$A$1000,Melbourne!A49)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N49" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M49,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O49" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M49,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P49" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M49,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q49" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M49,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R49" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A49,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S49" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A49,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -1413,6 +2675,30 @@
         <f>IF(COUNTIF(RosterOutput!A50:$A$1000,Melbourne!A50)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N50" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M50,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O50" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M50,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P50" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M50,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q50" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M50,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R50" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A50,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S50" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A50,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -1426,6 +2712,30 @@
         <f>IF(COUNTIF(RosterOutput!A51:$A$1000,Melbourne!A51)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N51" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M51,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O51" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M51,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P51" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M51,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q51" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M51,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R51" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A51,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S51" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A51,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -1439,6 +2749,30 @@
         <f>IF(COUNTIF(RosterOutput!A52:$A$1000,Melbourne!A52)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N52" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M52,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O52" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M52,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P52" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M52,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q52" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M52,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R52" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A52,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S52" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A52,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -1452,6 +2786,30 @@
         <f>IF(COUNTIF(RosterOutput!A53:$A$1000,Melbourne!A53)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N53" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M53,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O53" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M53,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P53" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M53,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q53" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M53,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R53" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A53,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S53" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A53,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -1465,6 +2823,30 @@
         <f>IF(COUNTIF(RosterOutput!A54:$A$1000,Melbourne!A54)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N54" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M54,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O54" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M54,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P54" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M54,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q54" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M54,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R54" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A54,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S54" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A54,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -1478,6 +2860,30 @@
         <f>IF(COUNTIF(RosterOutput!A55:$A$1000,Melbourne!A55)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N55" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M55,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O55" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M55,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P55" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M55,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q55" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M55,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R55" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A55,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S55" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A55,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -1491,6 +2897,30 @@
         <f>IF(COUNTIF(RosterOutput!A56:$A$1000,Melbourne!A56)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N56" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M56,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O56" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M56,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P56" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M56,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q56" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M56,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R56" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A56,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S56" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A56,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -1504,6 +2934,30 @@
         <f>IF(COUNTIF(RosterOutput!A57:$A$1000,Melbourne!A57)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N57" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M57,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O57" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M57,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P57" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M57,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q57" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M57,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R57" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A57,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S57" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A57,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -1517,6 +2971,30 @@
         <f>IF(COUNTIF(RosterOutput!A58:$A$1000,Melbourne!A58)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N58" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M58,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O58" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M58,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P58" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M58,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q58" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M58,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R58" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A58,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S58" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A58,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -1530,6 +3008,30 @@
         <f>IF(COUNTIF(RosterOutput!A59:$A$1000,Melbourne!A59)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N59" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M59,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O59" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M59,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P59" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M59,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q59" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M59,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R59" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A59,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S59" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A59,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -1543,6 +3045,30 @@
         <f>IF(COUNTIF(RosterOutput!A60:$A$1000,Melbourne!A60)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N60" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M60,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O60" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M60,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P60" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M60,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q60" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M60,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R60" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A60,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S60" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A60,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -1556,6 +3082,30 @@
         <f>IF(COUNTIF(RosterOutput!A61:$A$1000,Melbourne!A61)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N61" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M61,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O61" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M61,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P61" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M61,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q61" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M61,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R61" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A61,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S61" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A61,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -1569,6 +3119,30 @@
         <f>IF(COUNTIF(RosterOutput!A62:$A$1000,Melbourne!A62)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N62" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M62,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O62" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M62,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P62" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M62,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q62" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M62,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R62" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A62,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S62" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A62,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -1582,6 +3156,30 @@
         <f>IF(COUNTIF(RosterOutput!A63:$A$1000,Melbourne!A63)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N63" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M63,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O63" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M63,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P63" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M63,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q63" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M63,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R63" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A63,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S63" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A63,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -1595,6 +3193,30 @@
         <f>IF(COUNTIF(RosterOutput!A64:$A$1000,Melbourne!A64)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N64" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M64,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O64" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M64,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P64" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M64,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q64" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M64,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R64" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A64,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S64" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A64,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -1608,6 +3230,30 @@
         <f>IF(COUNTIF(RosterOutput!A65:$A$1000,Melbourne!A65)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N65" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M65,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O65" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M65,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P65" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M65,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q65" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M65,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R65" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A65,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S65" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A65,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -1621,6 +3267,30 @@
         <f>IF(COUNTIF(RosterOutput!A66:$A$1000,Melbourne!A66)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N66" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M66,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O66" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M66,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P66" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M66,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q66" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M66,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R66" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A66,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S66" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A66,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -1634,6 +3304,30 @@
         <f>IF(COUNTIF(RosterOutput!A67:$A$1000,Melbourne!A67)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N67" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M67,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O67" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M67,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P67" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M67,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q67" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M67,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R67" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A67,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S67" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A67,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -1647,6 +3341,30 @@
         <f>IF(COUNTIF(RosterOutput!A68:$A$1000,Melbourne!A68)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N68" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M68,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O68" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M68,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P68" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M68,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q68" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M68,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R68" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A68,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S68" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A68,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -1660,6 +3378,30 @@
         <f>IF(COUNTIF(RosterOutput!A69:$A$1000,Melbourne!A69)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N69" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M69,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O69" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M69,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P69" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M69,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q69" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M69,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R69" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A69,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S69" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A69,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -1673,6 +3415,30 @@
         <f>IF(COUNTIF(RosterOutput!A70:$A$1000,Melbourne!A70)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N70" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M70,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O70" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M70,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P70" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M70,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q70" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M70,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R70" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A70,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S70" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A70,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -1686,6 +3452,30 @@
         <f>IF(COUNTIF(RosterOutput!A71:$A$1000,Melbourne!A71)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N71" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M71,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O71" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M71,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P71" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M71,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q71" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M71,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R71" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A71,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S71" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A71,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -1699,6 +3489,30 @@
         <f>IF(COUNTIF(RosterOutput!A72:$A$1000,Melbourne!A72)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N72" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M72,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O72" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M72,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P72" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M72,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q72" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M72,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R72" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A72,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S72" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A72,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -1712,6 +3526,30 @@
         <f>IF(COUNTIF(RosterOutput!A73:$A$1000,Melbourne!A73)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N73" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M73,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O73" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M73,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P73" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M73,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q73" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M73,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R73" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A73,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S73" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A73,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -1725,6 +3563,30 @@
         <f>IF(COUNTIF(RosterOutput!A74:$A$1000,Melbourne!A74)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N74" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M74,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O74" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M74,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P74" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M74,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q74" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M74,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R74" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A74,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S74" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A74,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -1738,6 +3600,30 @@
         <f>IF(COUNTIF(RosterOutput!A75:$A$1000,Melbourne!A75)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N75" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M75,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O75" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M75,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P75" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M75,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q75" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M75,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R75" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A75,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S75" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A75,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -1751,6 +3637,30 @@
         <f>IF(COUNTIF(RosterOutput!A76:$A$1000,Melbourne!A76)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N76" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M76,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O76" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M76,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P76" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M76,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q76" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M76,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R76" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A76,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S76" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A76,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -1764,6 +3674,30 @@
         <f>IF(COUNTIF(RosterOutput!A77:$A$1000,Melbourne!A77)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N77" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M77,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O77" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M77,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P77" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M77,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q77" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M77,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R77" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A77,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S77" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A77,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -1777,6 +3711,30 @@
         <f>IF(COUNTIF(RosterOutput!A78:$A$1000,Melbourne!A78)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N78" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M78,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O78" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M78,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P78" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M78,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q78" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M78,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R78" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A78,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S78" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A78,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79">
@@ -1790,6 +3748,30 @@
         <f>IF(COUNTIF(RosterOutput!A79:$A$1000,Melbourne!A79)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N79" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M79,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O79" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M79,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P79" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M79,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q79" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M79,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R79" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A79,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S79" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A79,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80">
@@ -1803,6 +3785,30 @@
         <f>IF(COUNTIF(RosterOutput!A80:$A$1000,Melbourne!A80)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N80" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M80,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O80" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M80,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P80" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M80,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q80" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M80,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R80" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A80,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S80" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A80,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81">
@@ -1816,6 +3822,30 @@
         <f>IF(COUNTIF(RosterOutput!A81:$A$1000,Melbourne!A81)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N81" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M81,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O81" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M81,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P81" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M81,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q81" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M81,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R81" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A81,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S81" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A81,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82">
@@ -1829,6 +3859,30 @@
         <f>IF(COUNTIF(RosterOutput!A82:$A$1000,Melbourne!A82)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N82" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M82,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O82" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M82,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P82" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M82,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q82" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M82,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R82" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A82,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S82" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A82,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83">
@@ -1842,6 +3896,30 @@
         <f>IF(COUNTIF(RosterOutput!A83:$A$1000,Melbourne!A83)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N83" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M83,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O83" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M83,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P83" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M83,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q83" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M83,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R83" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A83,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S83" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A83,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84">
@@ -1855,6 +3933,30 @@
         <f>IF(COUNTIF(RosterOutput!A84:$A$1000,Melbourne!A84)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N84" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M84,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O84" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M84,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P84" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M84,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q84" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M84,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R84" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A84,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S84" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A84,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -1868,6 +3970,30 @@
         <f>IF(COUNTIF(RosterOutput!A85:$A$1000,Melbourne!A85)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N85" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M85,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O85" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M85,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P85" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M85,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q85" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M85,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R85" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A85,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S85" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A85,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -1881,6 +4007,30 @@
         <f>IF(COUNTIF(RosterOutput!A86:$A$1000,Melbourne!A86)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N86" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M86,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O86" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M86,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P86" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M86,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q86" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M86,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R86" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A86,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S86" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A86,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -1894,6 +4044,30 @@
         <f>IF(COUNTIF(RosterOutput!A87:$A$1000,Melbourne!A87)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N87" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M87,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O87" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M87,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P87" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M87,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q87" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M87,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R87" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A87,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S87" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A87,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -1907,6 +4081,30 @@
         <f>IF(COUNTIF(RosterOutput!A88:$A$1000,Melbourne!A88)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N88" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M88,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O88" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M88,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P88" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M88,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q88" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M88,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R88" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A88,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S88" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A88,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -1920,6 +4118,30 @@
         <f>IF(COUNTIF(RosterOutput!A89:$A$1000,Melbourne!A89)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N89" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M89,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O89" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M89,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P89" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M89,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q89" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M89,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R89" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A89,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S89" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A89,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -1933,6 +4155,30 @@
         <f>IF(COUNTIF(RosterOutput!A90:$A$1000,Melbourne!A90)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N90" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M90,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O90" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M90,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P90" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M90,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q90" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M90,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R90" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A90,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S90" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A90,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -1946,6 +4192,30 @@
         <f>IF(COUNTIF(RosterOutput!A91:$A$1000,Melbourne!A91)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N91" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M91,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O91" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M91,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P91" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M91,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q91" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M91,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R91" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A91,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S91" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A91,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -1959,6 +4229,30 @@
         <f>IF(COUNTIF(RosterOutput!A92:$A$1000,Melbourne!A92)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N92" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M92,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O92" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M92,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P92" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M92,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q92" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M92,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R92" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A92,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S92" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A92,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -1972,6 +4266,30 @@
         <f>IF(COUNTIF(RosterOutput!A93:$A$1000,Melbourne!A93)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N93" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M93,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O93" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M93,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P93" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M93,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q93" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M93,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R93" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A93,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S93" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A93,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94">
@@ -1985,6 +4303,30 @@
         <f>IF(COUNTIF(RosterOutput!A94:$A$1000,Melbourne!A94)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N94" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M94,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O94" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M94,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P94" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M94,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q94" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M94,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R94" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A94,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S94" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A94,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -1998,6 +4340,30 @@
         <f>IF(COUNTIF(RosterOutput!A95:$A$1000,Melbourne!A95)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N95" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M95,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O95" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M95,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P95" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M95,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q95" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M95,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R95" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A95,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S95" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A95,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -2011,6 +4377,30 @@
         <f>IF(COUNTIF(RosterOutput!A96:$A$1000,Melbourne!A96)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N96" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M96,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O96" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M96,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P96" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M96,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q96" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M96,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R96" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A96,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S96" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A96,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97">
@@ -2024,6 +4414,30 @@
         <f>IF(COUNTIF(RosterOutput!A97:$A$1000,Melbourne!A97)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N97" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M97,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O97" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M97,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P97" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M97,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q97" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M97,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R97" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A97,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S97" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A97,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98">
@@ -2037,6 +4451,30 @@
         <f>IF(COUNTIF(RosterOutput!A98:$A$1000,Melbourne!A98)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N98" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M98,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O98" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M98,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P98" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M98,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q98" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M98,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R98" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A98,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S98" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A98,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99">
@@ -2050,6 +4488,30 @@
         <f>IF(COUNTIF(RosterOutput!A99:$A$1000,Melbourne!A99)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N99" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M99,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O99" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M99,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P99" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M99,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q99" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M99,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R99" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A99,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S99" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A99,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100">
@@ -2063,6 +4525,30 @@
         <f>IF(COUNTIF(RosterOutput!A100:$A$1000,Melbourne!A100)&gt;1,"Rostered","Pending")</f>
         <v>Pending</v>
       </c>
+      <c r="N100" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M100,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O100" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M100,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P100" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M100,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q100" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M100,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R100" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A100,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S100" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A100,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101">
@@ -2074,6 +4560,30 @@
       </c>
       <c r="E101" t="str">
         <f>IF(COUNTIF(RosterOutput!A101:$A$1000,Melbourne!A101)&gt;1,"Rostered","Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="N101" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M101,'Contact Information'!$A$3:$A$628,0),MATCH(N$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="O101" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M101,'Contact Information'!$A$3:$A$628,0),MATCH(O$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="P101" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M101,'Contact Information'!$A$3:$A$628,0),MATCH(P$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="Q101" t="str">
+        <f>IFERROR(INDEX('Contact Information'!$A$3:$E$628,MATCH(Melbourne!$M101,'Contact Information'!$A$3:$A$628,0),MATCH(Q$1,'Contact Information'!$A$2:$E$2,0)),"")</f>
+        <v/>
+      </c>
+      <c r="R101" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$B$2:$B$10000,MATCH(Melbourne!$A101,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
+        <v>Pending</v>
+      </c>
+      <c r="S101" t="str">
+        <f>IFERROR(INDEX(RosterOutput!$C$2:$C$10000,MATCH(Melbourne!$A101,RosterOutput!$A$2:$A$10000,0),1),"Pending")</f>
         <v>Pending</v>
       </c>
     </row>

</xml_diff>